<commit_message>
Added ability to erase files in CP/M image. Massive code cleanup effort
</commit_message>
<xml_diff>
--- a/DiskUtility/Notes/MS-DOS Disk Parameters.xlsx
+++ b/DiskUtility/Notes/MS-DOS Disk Parameters.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\Github\DiskImageUtility\DiskUtility\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E6E2E1-FE6A-4FDD-AD26-FE1688100815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0073BB-06B7-4F39-B1FA-E4904C514181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="0" windowWidth="26085" windowHeight="14925" xr2:uid="{DA721517-95B2-498D-8FEE-4E0D30CAB48C}"/>
+    <workbookView xWindow="40350" yWindow="3255" windowWidth="34065" windowHeight="19200" activeTab="2" xr2:uid="{DA721517-95B2-498D-8FEE-4E0D30CAB48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Formats" sheetId="1" r:id="rId1"/>
     <sheet name="Boot Sector" sheetId="2" r:id="rId2"/>
+    <sheet name="Disk Analysis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="158">
   <si>
     <t>List of floppy disk formats</t>
   </si>
@@ -565,12 +566,159 @@
   <si>
     <t>Max Fat</t>
   </si>
+  <si>
+    <t>FAT12</t>
+  </si>
+  <si>
+    <t>Directory entry 0x1A has cluster of subdirectory cluster</t>
+  </si>
+  <si>
+    <t>Disk</t>
+  </si>
+  <si>
+    <t>TC05.DOS.IMG</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Sub Dir: SYS</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>4e</t>
+  </si>
+  <si>
+    <t>DIR Cluster</t>
+  </si>
+  <si>
+    <t>A00</t>
+  </si>
+  <si>
+    <t>BPB+4 = 5</t>
+  </si>
+  <si>
+    <t>First Sector BIOS Parameter Block</t>
+  </si>
+  <si>
+    <t>Bytes/Sector</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Sec/Cluster</t>
+  </si>
+  <si>
+    <t>Reserved Sectors</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t># FAT</t>
+  </si>
+  <si>
+    <t>Root Dir Entries</t>
+  </si>
+  <si>
+    <t>Total Sectors</t>
+  </si>
+  <si>
+    <t>2d0</t>
+  </si>
+  <si>
+    <t>Media Descriptor</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>Sector/FAT</t>
+  </si>
+  <si>
+    <t>SPT</t>
+  </si>
+  <si>
+    <t># Heads</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>Large Sector Cnt</t>
+  </si>
+  <si>
+    <t>Sub Dir Cluster</t>
+  </si>
+  <si>
+    <t>Subdirectory cluster</t>
+  </si>
+  <si>
+    <t>Dir Start</t>
+  </si>
+  <si>
+    <t>Subdirectory offset</t>
+  </si>
+  <si>
+    <t>(Cluster-2) * sec/cluster * bytes/Sector + Dir Start  --  start from 0</t>
+  </si>
+  <si>
+    <t>2f</t>
+  </si>
+  <si>
+    <t>Subdir</t>
+  </si>
+  <si>
+    <t>Math.h</t>
+  </si>
+  <si>
+    <t>cc00</t>
+  </si>
+  <si>
+    <t>Cluster * sec/cluster * bytes/Sector --  start from 0</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t># Sector</t>
+  </si>
+  <si>
+    <t>BPB</t>
+  </si>
+  <si>
+    <t>FAT 1</t>
+  </si>
+  <si>
+    <t>FAT 2</t>
+  </si>
+  <si>
+    <t>FAT</t>
+  </si>
+  <si>
+    <t>Sector size</t>
+  </si>
+  <si>
+    <t>Sectors per cluster</t>
+  </si>
+  <si>
+    <t>ZDOS3 320K</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -706,6 +854,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -803,7 +958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -824,12 +979,8 @@
     <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -843,7 +994,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -878,6 +1028,19 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -920,7 +1083,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -930,7 +1093,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9B8EFE5-905B-D707-691A-C51943776F83}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -980,7 +1143,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD9F521A-47FE-93D0-F7A4-4E4BD7532563}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1310,11 +1473,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:W1048576"/>
+      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,7 +1485,7 @@
     <col min="1" max="1" width="21.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="12"/>
+    <col min="4" max="4" width="9.140625" style="10"/>
     <col min="5" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
@@ -1338,7 +1501,7 @@
       </c>
       <c r="B1"/>
       <c r="C1"/>
-      <c r="D1" s="11"/>
+      <c r="D1" s="9"/>
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
@@ -1352,7 +1515,7 @@
       <c r="A2" s="3"/>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="D2" s="11"/>
+      <c r="D2" s="9"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
@@ -1363,20 +1526,20 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
     </row>
     <row r="4" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1421,7 +1584,7 @@
       <c r="N4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="25" t="s">
         <v>107</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -1441,7 +1604,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1450,7 +1613,7 @@
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="5">
         <v>1</v>
       </c>
@@ -1477,7 +1640,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1486,7 +1649,7 @@
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="5">
         <v>2</v>
       </c>
@@ -1513,7 +1676,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1522,7 +1685,7 @@
       <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="5">
         <v>1</v>
       </c>
@@ -1549,7 +1712,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1558,7 +1721,7 @@
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="5">
         <v>2</v>
       </c>
@@ -1585,7 +1748,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1594,7 +1757,7 @@
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="5">
@@ -1633,7 +1796,7 @@
         <v>2</v>
       </c>
       <c r="Q9" s="1">
-        <f>INT(T9/P9)</f>
+        <f t="shared" ref="Q9:Q14" si="0">INT(T9/P9)</f>
         <v>315</v>
       </c>
       <c r="R9" s="1">
@@ -1650,7 +1813,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1659,7 +1822,7 @@
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="5">
@@ -1698,7 +1861,7 @@
         <v>2</v>
       </c>
       <c r="Q10" s="1">
-        <f>INT(T10/P10)</f>
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
       <c r="R10" s="1">
@@ -1710,12 +1873,12 @@
         <v>140</v>
       </c>
       <c r="T10" s="1">
-        <f t="shared" ref="T10:T14" si="0">R10-(1+M10*2+O10)</f>
+        <f t="shared" ref="T10:T14" si="1">R10-(1+M10*2+O10)</f>
         <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1724,7 +1887,7 @@
       <c r="C11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="5">
@@ -1763,24 +1926,24 @@
         <v>1</v>
       </c>
       <c r="Q11" s="1">
-        <f>INT(T11/P11)</f>
-        <v>2371</v>
-      </c>
-      <c r="R11" s="1">
-        <f t="shared" ref="R11:R14" si="1">E11*F11*G11</f>
-        <v>2400</v>
-      </c>
-      <c r="S11" s="1" t="str">
-        <f t="shared" ref="S11:S14" si="2">DEC2HEX(R11)</f>
-        <v>960</v>
-      </c>
-      <c r="T11" s="1">
         <f t="shared" si="0"/>
         <v>2371</v>
       </c>
+      <c r="R11" s="1">
+        <f t="shared" ref="R11:R14" si="2">E11*F11*G11</f>
+        <v>2400</v>
+      </c>
+      <c r="S11" s="1" t="str">
+        <f t="shared" ref="S11:S14" si="3">DEC2HEX(R11)</f>
+        <v>960</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="1"/>
+        <v>2371</v>
+      </c>
     </row>
     <row r="12" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1789,7 +1952,7 @@
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="5">
@@ -1818,7 +1981,7 @@
         <v>2</v>
       </c>
       <c r="N12" s="1" t="str">
-        <f t="shared" ref="N12:N14" si="3">DEC2HEX((1+M12*2)*H12)</f>
+        <f t="shared" ref="N12:N14" si="4">DEC2HEX((1+M12*2)*H12)</f>
         <v>A00</v>
       </c>
       <c r="O12" s="1">
@@ -1828,24 +1991,24 @@
         <v>2</v>
       </c>
       <c r="Q12" s="1">
-        <f>INT(T12/P12)</f>
+        <f t="shared" si="0"/>
         <v>354</v>
       </c>
       <c r="R12" s="1">
+        <f t="shared" si="2"/>
+        <v>720</v>
+      </c>
+      <c r="S12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>2D0</v>
+      </c>
+      <c r="T12" s="1">
         <f t="shared" si="1"/>
-        <v>720</v>
-      </c>
-      <c r="S12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>2D0</v>
-      </c>
-      <c r="T12" s="1">
-        <f t="shared" si="0"/>
         <v>708</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1854,7 +2017,7 @@
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="5">
@@ -1883,7 +2046,7 @@
         <v>2</v>
       </c>
       <c r="N13" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>A00</v>
       </c>
       <c r="O13" s="1">
@@ -1893,24 +2056,24 @@
         <v>2</v>
       </c>
       <c r="Q13" s="1">
-        <f>INT(T13/P13)</f>
+        <f t="shared" si="0"/>
         <v>714</v>
       </c>
       <c r="R13" s="1">
+        <f t="shared" si="2"/>
+        <v>1440</v>
+      </c>
+      <c r="S13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>5A0</v>
+      </c>
+      <c r="T13" s="1">
         <f t="shared" si="1"/>
-        <v>1440</v>
-      </c>
-      <c r="S13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>5A0</v>
-      </c>
-      <c r="T13" s="1">
-        <f t="shared" si="0"/>
         <v>1428</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1919,7 +2082,7 @@
       <c r="C14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="5">
@@ -1948,7 +2111,7 @@
         <v>9</v>
       </c>
       <c r="N14" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2600</v>
       </c>
       <c r="O14" s="1">
@@ -1958,24 +2121,24 @@
         <v>1</v>
       </c>
       <c r="Q14" s="1">
-        <f>INT(T14/P14)</f>
-        <v>2847</v>
-      </c>
-      <c r="R14" s="1">
-        <f t="shared" si="1"/>
-        <v>2880</v>
-      </c>
-      <c r="S14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>B40</v>
-      </c>
-      <c r="T14" s="1">
         <f t="shared" si="0"/>
         <v>2847</v>
       </c>
+      <c r="R14" s="1">
+        <f t="shared" si="2"/>
+        <v>2880</v>
+      </c>
+      <c r="S14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>B40</v>
+      </c>
+      <c r="T14" s="1">
+        <f t="shared" si="1"/>
+        <v>2847</v>
+      </c>
     </row>
     <row r="15" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1984,7 +2147,7 @@
       <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="5">
         <v>1</v>
       </c>
@@ -2009,7 +2172,7 @@
       <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2018,7 +2181,7 @@
       <c r="C16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="5">
         <v>1</v>
       </c>
@@ -2043,7 +2206,7 @@
       <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -2052,7 +2215,7 @@
       <c r="C17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="5">
         <v>2</v>
       </c>
@@ -2077,7 +2240,7 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -2086,7 +2249,7 @@
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="5">
         <v>1</v>
       </c>
@@ -2111,7 +2274,7 @@
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -2120,7 +2283,7 @@
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="5">
         <v>1</v>
       </c>
@@ -2145,7 +2308,7 @@
       <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -2154,7 +2317,7 @@
       <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="5">
         <v>2</v>
       </c>
@@ -2179,7 +2342,7 @@
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -2188,7 +2351,7 @@
       <c r="C21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="5">
         <v>2</v>
       </c>
@@ -2210,12 +2373,12 @@
       <c r="K21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="L21" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -2224,7 +2387,7 @@
       <c r="C22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="5">
         <v>2</v>
       </c>
@@ -2246,12 +2409,12 @@
       <c r="K22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="L22" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -2260,7 +2423,7 @@
       <c r="C23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="5">
         <v>2</v>
       </c>
@@ -2318,7 +2481,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId25" name="Control 3">
+        <control shapeId="1026" r:id="rId25" name="Control 2">
           <controlPr defaultSize="0" r:id="rId26">
             <anchor moveWithCells="1">
               <from>
@@ -2338,13 +2501,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId25" name="Control 3"/>
+        <control shapeId="1026" r:id="rId25" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId27" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId28">
+        <control shapeId="1027" r:id="rId27" name="Control 3">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId26">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -2356,14 +2519,14 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>2</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId27" name="Control 2"/>
+        <control shapeId="1027" r:id="rId27" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2375,291 +2538,851 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="15"/>
     <col min="2" max="2" width="90.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:2" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="24">
+      <c r="A8" s="21">
         <v>10</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="20" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
+      <c r="A11" s="21">
         <v>15</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="20" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="20" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="20" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
+      <c r="B26" s="24"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="23" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="23" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="23" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="23" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="23" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="23" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="23" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="23" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="23" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
+      <c r="B36" s="24"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="23" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="23" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="23" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="23" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="23" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="23" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="23" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="27"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="23" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="23" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
+      <c r="B47" s="24"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="23" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="23" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="23" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B51" s="18"/>
+      <c r="B51" s="15"/>
     </row>
     <row r="52" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="15" t="s">
         <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30585092-C7EC-4AB8-BE40-1974892A337D}">
+  <dimension ref="B2:W28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2">
+        <v>14800</v>
+      </c>
+      <c r="M2" t="s">
+        <v>145</v>
+      </c>
+      <c r="N2" s="29">
+        <v>52</v>
+      </c>
+      <c r="P2" s="29">
+        <v>14800</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" t="s">
+        <v>146</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="P3" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="V3">
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T4" s="29">
+        <v>4656</v>
+      </c>
+      <c r="U4" s="29" t="str">
+        <f>DEC2HEX(T4)</f>
+        <v>1230</v>
+      </c>
+      <c r="V4">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" t="s">
+        <v>113</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="V5">
+        <f>V3/V4</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="U6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="V6" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="W6" s="30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="29">
+        <f t="shared" ref="F7:F8" si="0">HEX2DEC(E7)</f>
+        <v>78</v>
+      </c>
+      <c r="G7">
+        <f>F7*$F$14*$F$13+$F$8</f>
+        <v>82432</v>
+      </c>
+      <c r="H7" s="29" t="str">
+        <f>DEC2HEX(G7)</f>
+        <v>14200</v>
+      </c>
+      <c r="O7" s="29">
+        <f>O10*$F$14*$F$13+$F$8</f>
+        <v>50688</v>
+      </c>
+      <c r="T7" s="29">
+        <v>1000</v>
+      </c>
+      <c r="U7" s="29">
+        <f>HEX2DEC(T7)</f>
+        <v>4096</v>
+      </c>
+      <c r="V7" s="29">
+        <v>512</v>
+      </c>
+      <c r="W7">
+        <f>U7/V7</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="29">
+        <f t="shared" si="0"/>
+        <v>2560</v>
+      </c>
+      <c r="J8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8">
+        <f>5*512</f>
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>F8/1024</f>
+        <v>2.5</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="O9" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="M10" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="N10" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="O10" s="29">
+        <f>HEX2DEC(N10)</f>
+        <v>47</v>
+      </c>
+      <c r="P10" s="29" t="str">
+        <f>DEC2HEX(O10)</f>
+        <v>2F</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" t="s">
+        <v>157</v>
+      </c>
+      <c r="M11" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="O11" s="29">
+        <v>2</v>
+      </c>
+      <c r="P11" s="29" t="str">
+        <f t="shared" ref="P11:P16" si="1">DEC2HEX(O11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D12" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="O12" s="29">
+        <v>512</v>
+      </c>
+      <c r="P12" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="29">
+        <v>200</v>
+      </c>
+      <c r="F13" s="29">
+        <f>HEX2DEC(E13)</f>
+        <v>512</v>
+      </c>
+      <c r="G13" s="29">
+        <v>200</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="N13" s="29">
+        <v>1800</v>
+      </c>
+      <c r="O13" s="29">
+        <f>HEX2DEC(N13)</f>
+        <v>6144</v>
+      </c>
+      <c r="P13" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="29">
+        <v>2</v>
+      </c>
+      <c r="F14" s="29">
+        <f t="shared" ref="F14:F24" si="2">HEX2DEC(E14)</f>
+        <v>2</v>
+      </c>
+      <c r="G14" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="29">
+        <v>1</v>
+      </c>
+      <c r="F15" s="29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="29">
+        <v>1</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="O15" s="29">
+        <f>O10*O11*O12</f>
+        <v>48128</v>
+      </c>
+      <c r="P15" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>BC00</v>
+      </c>
+      <c r="R15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="29">
+        <v>10</v>
+      </c>
+      <c r="E16" s="29">
+        <v>2</v>
+      </c>
+      <c r="F16" s="29">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="29">
+        <v>2</v>
+      </c>
+      <c r="O16" s="29">
+        <f>(O10-2)*O11*O12+O13</f>
+        <v>52224</v>
+      </c>
+      <c r="P16" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>CC00</v>
+      </c>
+      <c r="R16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="29">
+        <v>11</v>
+      </c>
+      <c r="E17" s="29">
+        <v>70</v>
+      </c>
+      <c r="F17" s="29">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="G17" s="29">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="29">
+        <v>13</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="29">
+        <f t="shared" si="2"/>
+        <v>720</v>
+      </c>
+      <c r="G18" s="29">
+        <v>280</v>
+      </c>
+      <c r="I18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="29">
+        <v>15</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="29">
+        <f t="shared" si="2"/>
+        <v>253</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" t="s">
+        <v>152</v>
+      </c>
+      <c r="J19">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="29">
+        <v>16</v>
+      </c>
+      <c r="E20" s="29">
+        <v>2</v>
+      </c>
+      <c r="F20" s="29">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G20" s="29">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>153</v>
+      </c>
+      <c r="J20">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="29">
+        <v>18</v>
+      </c>
+      <c r="E21" s="29">
+        <v>9</v>
+      </c>
+      <c r="F21" s="29">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G21" s="29">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <f>SUM(J18:J20)</f>
+        <v>2560</v>
+      </c>
+      <c r="K21" s="29" t="str">
+        <f>DEC2HEX(J21)</f>
+        <v>A00</v>
+      </c>
+      <c r="O21" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="29">
+        <v>2</v>
+      </c>
+      <c r="F22" s="29">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G22" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="29">
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="29">
+        <v>20</v>
+      </c>
+      <c r="E24" s="29">
+        <v>0</v>
+      </c>
+      <c r="F24" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="J26">
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <f>SUM(J26:J27)</f>
+        <v>6144</v>
+      </c>
+      <c r="K28" s="29" t="str">
+        <f>DEC2HEX(J28)</f>
+        <v>1800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>